<commit_message>
Cambio 10 en excel
</commit_message>
<xml_diff>
--- a/src/test/resources/datos/DataExcel.xlsx
+++ b/src/test/resources/datos/DataExcel.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Desktop\PageObjectModel_Repaso\src\test\resources\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\Git\PageObjectModel_Repaso\src\test\resources\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE7D0A3-685B-4AF2-8797-2D4FCBFCDEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31296ADC-762C-4703-ACC8-92E6482DEB84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="DatosCP" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -146,12 +145,18 @@
   </si>
   <si>
     <t>Superaste el número de intentos y por seguridad bloqueamos tu cuenta. Espera 24 hrs e inténtalo nuevamente.</t>
+  </si>
+  <si>
+    <t>dato3CP3</t>
+  </si>
+  <si>
+    <t>qweqw    CAMBIO 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -532,7 +537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555B203E-51BE-43F9-82B1-F4C932530781}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
@@ -733,11 +738,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD81E873-3C2C-4C18-BD82-BD2C4789CCC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,10 +813,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -920,7 +925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3058DCD6-9B30-42B4-908B-80298340871D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>